<commit_message>
Handle interference without PUN
</commit_message>
<xml_diff>
--- a/data/data_final4.xlsx
+++ b/data/data_final4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Document\NTHU\master\Final\HRC_taskalloc_w.TB_w.AR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA185AF-EEE4-42CE-B811-6E3654D26CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40562A04-3C1D-42EE-BDDC-F4123C21A45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Therbligs1" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="43">
   <si>
     <t>From</t>
   </si>
@@ -149,16 +149,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>WP5_TOP</t>
-  </si>
-  <si>
     <t>DA5_TOP</t>
   </si>
   <si>
     <t>DA6_TOP</t>
-  </si>
-  <si>
-    <t>DA6</t>
   </si>
   <si>
     <t>A1_TOP</t>
@@ -184,6 +178,14 @@
   </si>
   <si>
     <t>BIN1_TOP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA5_TOP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP6</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -554,7 +556,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +651,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -662,10 +664,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -673,10 +675,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -741,7 +743,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>
@@ -754,10 +756,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -765,7 +767,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
@@ -779,10 +781,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -918,10 +920,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1234,10 +1236,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1448,10 +1450,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,7 +1488,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1497,10 +1499,10 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1508,10 +1510,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -1519,38 +1521,39 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1558,78 +1561,67 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -1637,12 +1629,12 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
@@ -1658,10 +1650,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
+      <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
@@ -1671,10 +1663,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
+      <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
@@ -1684,10 +1676,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
+      <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -1697,10 +1689,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
+      <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
@@ -1713,6 +1705,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
+      <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
@@ -1720,7 +1713,6 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
@@ -1733,23 +1725,20 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
+      <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
+      <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1766,7 +1755,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,7 +1850,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1874,10 +1863,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,10 +1874,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1953,7 +1942,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>
@@ -1966,10 +1955,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,7 +1966,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
@@ -1994,7 +1983,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2135,7 +2124,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2351,8 +2340,8 @@
   </sheetPr>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,7 +2443,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>